<commit_message>
Added logging for sessions, added session7 data
</commit_message>
<xml_diff>
--- a/data/Prompts_Utterances.xlsx
+++ b/data/Prompts_Utterances.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="official" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="in progress" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="98">
   <si>
     <t>Situation</t>
   </si>
@@ -100,37 +101,37 @@
     <t>I don't</t>
   </si>
   <si>
-    <t>I have no idea</t>
-  </si>
-  <si>
-    <t>I don't think so</t>
-  </si>
-  <si>
-    <t>I hope so</t>
-  </si>
-  <si>
-    <t>I'm sorry</t>
-  </si>
-  <si>
-    <t>I'm sorry to hear that</t>
-  </si>
-  <si>
-    <t>Thank you</t>
-  </si>
-  <si>
-    <t>I understand that</t>
-  </si>
-  <si>
-    <t>I went through something similar</t>
-  </si>
-  <si>
-    <t>I am not sure</t>
-  </si>
-  <si>
-    <t>I can't hear you</t>
-  </si>
-  <si>
-    <t>I don't understand</t>
+    <t>I have no idea.</t>
+  </si>
+  <si>
+    <t>I don't think so.</t>
+  </si>
+  <si>
+    <t>I hope so.</t>
+  </si>
+  <si>
+    <t>I'm sorry.</t>
+  </si>
+  <si>
+    <t>I'm sorry to hear that.</t>
+  </si>
+  <si>
+    <t>Thank you.</t>
+  </si>
+  <si>
+    <t>I understand that.</t>
+  </si>
+  <si>
+    <t>I went through something similar.</t>
+  </si>
+  <si>
+    <t>I am not sure.</t>
+  </si>
+  <si>
+    <t>I can't hear you.</t>
+  </si>
+  <si>
+    <t>I don't understand.</t>
   </si>
   <si>
     <t>Can you repeat that?</t>
@@ -145,7 +146,7 @@
     <t>Can you ask me something else?</t>
   </si>
   <si>
-    <t>It would help if you could keep the questions short and simple</t>
+    <t>It would help if you could keep the questions short and simple.</t>
   </si>
   <si>
     <t>Can you rephrase the question?</t>
@@ -157,22 +158,22 @@
     <t>I do not want to speculate about the future.</t>
   </si>
   <si>
-    <t>I don't know what that is</t>
-  </si>
-  <si>
-    <t>I don't know who that is</t>
-  </si>
-  <si>
-    <t>I am not going to talk about that</t>
-  </si>
-  <si>
-    <t>I am not here to talk about that</t>
+    <t>I don't know what that is.</t>
+  </si>
+  <si>
+    <t>I don't know who that is.</t>
+  </si>
+  <si>
+    <t>I am not going to talk about that.</t>
+  </si>
+  <si>
+    <t>I am not here to talk about that.</t>
   </si>
   <si>
     <t>Anything else?</t>
   </si>
   <si>
-    <t>I don't have enough information to talk about that</t>
+    <t>I don't have enough information to talk about that.</t>
   </si>
   <si>
     <t>I do not have an answer for that.</t>
@@ -181,7 +182,7 @@
     <t>_OFF_TOPIC_</t>
   </si>
   <si>
-    <t>That is a great question, unfortunately I never recorded an answer to that.</t>
+    <t>That is a great question, but unfortunately I never recorded an answer to that.</t>
   </si>
   <si>
     <t>That is a great question. I wish I'd thought of that.</t>
@@ -190,7 +191,7 @@
     <t xml:space="preserve">That is an interesting question, but I am here to talk about STEM careers in the Navy. </t>
   </si>
   <si>
-    <t>Unfortunately I was never asked that question</t>
+    <t>Unfortunately, I was never asked that question.</t>
   </si>
   <si>
     <t>You might have to ask me something else.</t>
@@ -253,7 +254,7 @@
     <t>Good careers are about solving what's important. You can ask me about anything that I think is important.</t>
   </si>
   <si>
-    <t>I am stored in this machine, I can wait for your questions all day</t>
+    <t>I am stored in this machine, I can wait for your questions all day.</t>
   </si>
   <si>
     <t>Do you have any more questions for me?</t>
@@ -271,19 +272,40 @@
     <t>I have already answered that question. Please ask me something else.</t>
   </si>
   <si>
-    <t>I have answered that question before. You can ask me something else</t>
+    <t>I have answered that question before. You can ask me something else.</t>
   </si>
   <si>
     <t>I answered this question a while ago. Let’s move on.</t>
   </si>
   <si>
-    <t>That's a great question. Unfortunately, I don't have an answer for that right now.</t>
+    <t>That's a great question, but unfortunately, I don't have an answer for that right now.</t>
   </si>
   <si>
     <t>I'm not sure I have an answer for that question.</t>
   </si>
   <si>
-    <t>That is a great question but unfortunately, I don't have an answer right now</t>
+    <t>That is a great question but unfortunately, I don't have an answer right now.</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>It's nice to meet you.</t>
+  </si>
+  <si>
+    <t>Can you please refrain from the use of profanity?</t>
+  </si>
+  <si>
+    <t>I don't really have an opinion on that.</t>
+  </si>
+  <si>
+    <t>I see you didn't ask me anything there.</t>
+  </si>
+  <si>
+    <t>You've got to ask me something to get a response.</t>
+  </si>
+  <si>
+    <t>No matter what you heard about having a mouth like a sailor, it will hurt your career.</t>
   </si>
 </sst>
 </file>
@@ -336,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -349,10 +371,19 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -373,6 +404,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
@@ -645,7 +680,7 @@
       <c r="B24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -656,7 +691,7 @@
       <c r="B25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -667,7 +702,7 @@
       <c r="B26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -678,7 +713,7 @@
       <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -689,7 +724,7 @@
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -700,7 +735,7 @@
       <c r="B29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -711,7 +746,7 @@
       <c r="B30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -722,7 +757,7 @@
       <c r="B31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -733,7 +768,7 @@
       <c r="B32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -744,7 +779,7 @@
       <c r="B33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -755,7 +790,7 @@
       <c r="B34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -766,7 +801,7 @@
       <c r="B35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -810,7 +845,7 @@
       <c r="B39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -854,7 +889,7 @@
       <c r="B43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -865,7 +900,7 @@
       <c r="B44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -876,7 +911,7 @@
       <c r="B45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -887,7 +922,7 @@
       <c r="B46" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -909,7 +944,7 @@
       <c r="B48" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -920,7 +955,7 @@
       <c r="B49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="6" t="s">
         <v>54</v>
       </c>
     </row>
@@ -931,7 +966,7 @@
       <c r="B50" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -942,7 +977,7 @@
       <c r="B51" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="6" t="s">
         <v>57</v>
       </c>
     </row>
@@ -953,7 +988,7 @@
       <c r="B52" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -964,7 +999,7 @@
       <c r="B53" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="5" t="s">
         <v>59</v>
       </c>
     </row>
@@ -975,7 +1010,7 @@
       <c r="B54" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="6" t="s">
         <v>60</v>
       </c>
     </row>
@@ -986,7 +1021,7 @@
       <c r="B55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="6" t="s">
         <v>61</v>
       </c>
     </row>
@@ -997,7 +1032,7 @@
       <c r="B56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="6" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1008,7 +1043,7 @@
       <c r="B57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1019,7 +1054,7 @@
       <c r="B58" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1030,7 +1065,7 @@
       <c r="B59" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="6" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1041,7 +1076,7 @@
       <c r="B60" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="6" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1052,7 +1087,7 @@
       <c r="B61" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="6" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1063,7 +1098,7 @@
       <c r="B62" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1074,7 +1109,7 @@
       <c r="B63" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="6" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1085,7 +1120,7 @@
       <c r="B64" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="6" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1096,7 +1131,7 @@
       <c r="B65" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="7" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1107,7 +1142,7 @@
       <c r="B66" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="7" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1118,7 +1153,7 @@
       <c r="B67" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="7" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1129,7 +1164,7 @@
       <c r="B68" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="7" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1140,7 +1175,7 @@
       <c r="B69" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="7" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1151,7 +1186,7 @@
       <c r="B70" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1162,7 +1197,7 @@
       <c r="B71" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="8" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1173,7 +1208,7 @@
       <c r="B72" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="8" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1184,7 +1219,7 @@
       <c r="B73" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="8" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1195,7 +1230,7 @@
       <c r="B74" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C74" s="9" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1261,7 +1296,7 @@
       <c r="B80" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C80" s="4" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1283,7 +1318,7 @@
       <c r="B82" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C82" s="4" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1305,8 +1340,111 @@
       <c r="B84" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="C84" s="10" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="44.43"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>